<commit_message>
Change two empty rows
</commit_message>
<xml_diff>
--- a/template_baogia.xlsx
+++ b/template_baogia.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTG\Bao gia\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0321C54B-6F31-4122-B40F-1AC72987174C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3655FF81-5995-491F-95EB-4E253DF36B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1875" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Báo giá - Quotation" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Báo giá - Quotation'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Báo giá - Quotation'!$A$1:$K$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Báo giá - Quotation'!$A$1:$K$53</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -379,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -502,12 +502,69 @@
     <xf numFmtId="41" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -516,57 +573,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -967,10 +973,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A8" zoomScale="86" zoomScaleNormal="69" zoomScaleSheetLayoutView="78" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="86" zoomScaleNormal="69" zoomScaleSheetLayoutView="78" zoomScalePageLayoutView="86" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,19 +1079,19 @@
       <c r="V4" s="36"/>
     </row>
     <row r="5" spans="1:22" ht="33" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="T5" s="45"/>
@@ -1093,17 +1099,17 @@
       <c r="V5" s="36"/>
     </row>
     <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="T6" s="45"/>
@@ -1127,81 +1133,81 @@
       <c r="V7" s="37"/>
     </row>
     <row r="8" spans="1:22" s="5" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
     </row>
     <row r="9" spans="1:22" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
     </row>
     <row r="10" spans="1:22" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
     </row>
     <row r="11" spans="1:22" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
     </row>
     <row r="12" spans="1:22" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
     </row>
     <row r="13" spans="1:22" s="5" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28"/>
@@ -1217,19 +1223,19 @@
       <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:22" s="13" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
     </row>
     <row r="15" spans="1:22" s="20" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
@@ -1265,16 +1271,16 @@
       <c r="A17" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60" t="s">
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="60"/>
+      <c r="G17" s="65"/>
       <c r="H17" s="46" t="s">
         <v>5</v>
       </c>
@@ -1291,12 +1297,12 @@
     </row>
     <row r="18" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="J18" s="48"/>
@@ -1307,374 +1313,374 @@
       <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="49">
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="49">
         <f>SUM(K18:K18)</f>
         <v>0</v>
       </c>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="49">
-        <f>K19*10%</f>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="49">
+        <f>K20*10%</f>
         <v>0</v>
       </c>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="49">
-        <f>K19+K20</f>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="49">
+        <f>K20+K21</f>
         <v>0</v>
       </c>
-      <c r="L21" s="16"/>
-    </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
       <c r="L22" s="16"/>
     </row>
-    <row r="23" spans="1:12" s="5" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+    <row r="23" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="62"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
       <c r="L23" s="16"/>
     </row>
-    <row r="24" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59" t="s">
+    <row r="24" spans="1:12" s="5" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="19"/>
-    </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="19"/>
+    </row>
+    <row r="26" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59" t="s">
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="16"/>
+    </row>
+    <row r="27" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="19"/>
-    </row>
-    <row r="27" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="19"/>
+    </row>
+    <row r="28" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="16"/>
-    </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="s">
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="16"/>
+    </row>
+    <row r="29" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="16"/>
+    </row>
+    <row r="30" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="19"/>
-    </row>
-    <row r="30" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="s">
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="19"/>
+    </row>
+    <row r="31" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="34"/>
-    </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="65" t="s">
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="34"/>
+    </row>
+    <row r="32" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="16"/>
-    </row>
-    <row r="32" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="16"/>
+    </row>
+    <row r="33" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="19"/>
-    </row>
-    <row r="33" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="19"/>
+    </row>
+    <row r="34" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="16"/>
-    </row>
-    <row r="34" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59" t="s">
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="16"/>
+    </row>
+    <row r="35" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="19"/>
-    </row>
-    <row r="35" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="65" t="s">
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="19"/>
+    </row>
+    <row r="36" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="65"/>
-      <c r="L35" s="16"/>
-    </row>
-    <row r="36" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="65" t="s">
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="16"/>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="16"/>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="65" t="s">
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="16"/>
+    </row>
+    <row r="38" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="16"/>
-    </row>
-    <row r="38" spans="1:12" s="5" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
       <c r="L38" s="16"/>
     </row>
-    <row r="39" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51" t="s">
+    <row r="39" spans="1:12" s="5" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="16"/>
+    </row>
+    <row r="40" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="16"/>
-    </row>
-    <row r="40" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
+      <c r="H40" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
       <c r="L40" s="16"/>
     </row>
-    <row r="41" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="42"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23"/>
+    <row r="41" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="23"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
       <c r="L41" s="16"/>
     </row>
     <row r="42" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1734,146 +1740,146 @@
       <c r="L45" s="16"/>
     </row>
     <row r="46" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="69"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
-      <c r="H46" s="28"/>
+      <c r="H46" s="44"/>
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
-      <c r="K46" s="29"/>
+      <c r="K46" s="23"/>
       <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="69"/>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
-      <c r="H47" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="29"/>
       <c r="L47" s="16"/>
     </row>
-    <row r="48" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="71"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
+    <row r="48" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
-      <c r="H48" s="70"/>
-      <c r="I48" s="70"/>
-      <c r="J48" s="70"/>
-      <c r="K48" s="70"/>
+      <c r="H48" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="54"/>
       <c r="L48" s="16"/>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
+      <c r="A49" s="55"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
-      <c r="H49" s="70"/>
-      <c r="I49" s="70"/>
-      <c r="J49" s="70"/>
-      <c r="K49" s="70"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="54"/>
       <c r="L49" s="16"/>
     </row>
     <row r="50" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
-      <c r="H50" s="68" t="s">
-        <v>39</v>
-      </c>
-      <c r="I50" s="68"/>
-      <c r="J50" s="68"/>
-      <c r="K50" s="68"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
+      <c r="K50" s="54"/>
       <c r="L50" s="16"/>
     </row>
     <row r="51" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="68"/>
-      <c r="C51" s="68"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
+      <c r="A51" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="54"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="68" t="s">
+      <c r="H51" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="16"/>
+    </row>
+    <row r="52" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="52"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="I51" s="68"/>
-      <c r="J51" s="68"/>
-      <c r="K51" s="68"/>
-      <c r="L51" s="16"/>
-    </row>
-    <row r="52" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="68" t="s">
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="16"/>
+    </row>
+    <row r="53" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="68" t="s">
+      <c r="B53" s="52"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I52" s="68"/>
-      <c r="J52" s="68"/>
-      <c r="K52" s="68"/>
-      <c r="L52" s="16"/>
-    </row>
-    <row r="53" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
       <c r="L53" s="16"/>
     </row>
-    <row r="54" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
+    <row r="54" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
     </row>
     <row r="55" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11"/>
@@ -1983,11 +1989,12 @@
       <c r="G62" s="10"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
+      <c r="J62" s="9"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
     </row>
     <row r="63" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
@@ -2077,12 +2084,18 @@
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:12" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="12"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
+    <row r="70" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
     </row>
     <row r="71" spans="1:12" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
@@ -2154,91 +2167,98 @@
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="12"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="H47:K49"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="H39:K40"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="G12:K12"/>
     <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A19:J19"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="H40:K41"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="H48:K50"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="H51:K51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="10" orientation="portrait" r:id="rId1"/>
@@ -2260,12 +2280,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7683A1A7D7B9D498698F072A553A313" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a504a8be0005da0ec9b7c5289d45737">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d02630e-4ced-4d5b-a38c-7429e3dd9e77" xmlns:ns3="c5f625c1-6a31-4537-bcb6-f2e0024ec460" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="18d92fd5d13b4b498ebf6911e5bff178" ns2:_="" ns3:_="">
     <xsd:import namespace="5d02630e-4ced-4d5b-a38c-7429e3dd9e77"/>
@@ -2462,6 +2476,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66EDE61C-DACD-42B8-9F49-698A5DDB3ED9}">
   <ds:schemaRefs>
@@ -2471,15 +2491,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5022B6AC-8E94-40F2-9FFC-FC610C08F9CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A766724-5662-42F2-8CBB-A93D00C46B36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2496,4 +2507,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5022B6AC-8E94-40F2-9FFC-FC610C08F9CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change to 3 empty rows
</commit_message>
<xml_diff>
--- a/template_baogia.xlsx
+++ b/template_baogia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTG\Bao gia\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3655FF81-5995-491F-95EB-4E253DF36B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C767A5E-9D16-4299-ACE7-67DE53AA9C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="1875" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Báo giá - Quotation'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Báo giá - Quotation'!$A$1:$K$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Báo giá - Quotation'!$A$1:$K$54</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -973,10 +973,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:V93"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="86" zoomScaleNormal="69" zoomScaleSheetLayoutView="78" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,27 +1327,22 @@
       <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="49">
-        <f>SUM(K18:K18)</f>
-        <v>0</v>
-      </c>
+      <c r="A20" s="51"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
       <c r="L20" s="16"/>
     </row>
     <row r="21" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B21" s="61"/>
       <c r="C21" s="61"/>
@@ -1359,14 +1354,14 @@
       <c r="I21" s="61"/>
       <c r="J21" s="61"/>
       <c r="K21" s="49">
-        <f>K20*10%</f>
+        <f>SUM(K18:K18)</f>
         <v>0</v>
       </c>
       <c r="L21" s="16"/>
     </row>
     <row r="22" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B22" s="61"/>
       <c r="C22" s="61"/>
@@ -1378,234 +1373,237 @@
       <c r="I22" s="61"/>
       <c r="J22" s="61"/>
       <c r="K22" s="49">
-        <f>K20+K21</f>
+        <f>K21*10%</f>
         <v>0</v>
       </c>
       <c r="L22" s="16"/>
     </row>
     <row r="23" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
+      <c r="A23" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="49">
+        <f>K21+K22</f>
+        <v>0</v>
+      </c>
       <c r="L23" s="16"/>
     </row>
-    <row r="24" spans="1:12" s="5" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
+    <row r="24" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="62"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
       <c r="L24" s="16"/>
     </row>
-    <row r="25" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59" t="s">
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="16"/>
+    </row>
+    <row r="26" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="19"/>
-    </row>
-    <row r="26" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="19"/>
+    </row>
+    <row r="27" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="63"/>
-      <c r="L26" s="16"/>
-    </row>
-    <row r="27" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="59" t="s">
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="16"/>
+    </row>
+    <row r="28" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="19"/>
-    </row>
-    <row r="28" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="16"/>
+    </row>
+    <row r="30" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="16"/>
-    </row>
-    <row r="30" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="16"/>
+    </row>
+    <row r="31" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="19"/>
-    </row>
-    <row r="31" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="19"/>
+    </row>
+    <row r="32" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="34"/>
-    </row>
-    <row r="32" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="34"/>
+    </row>
+    <row r="33" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="16"/>
-    </row>
-    <row r="33" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="s">
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="16"/>
+    </row>
+    <row r="34" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="19"/>
-    </row>
-    <row r="34" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="19"/>
+    </row>
+    <row r="35" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="16"/>
-    </row>
-    <row r="35" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="59" t="s">
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="16"/>
+    </row>
+    <row r="36" spans="1:12" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="19"/>
-    </row>
-    <row r="36" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="19"/>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="57" t="s">
         <v>44</v>
-      </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="16"/>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
-        <v>45</v>
       </c>
       <c r="B37" s="57"/>
       <c r="C37" s="57"/>
@@ -1621,7 +1619,7 @@
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B38" s="57"/>
       <c r="C38" s="57"/>
@@ -1635,41 +1633,39 @@
       <c r="K38" s="57"/>
       <c r="L38" s="16"/>
     </row>
-    <row r="39" spans="1:12" s="5" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
+    <row r="39" spans="1:12" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
       <c r="L39" s="16"/>
     </row>
-    <row r="40" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
+    <row r="40" spans="1:12" s="5" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="41"/>
       <c r="L40" s="16"/>
     </row>
     <row r="41" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B41" s="56"/>
       <c r="C41" s="56"/>
@@ -1677,24 +1673,28 @@
       <c r="E41" s="56"/>
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
-      <c r="H41" s="56"/>
+      <c r="H41" s="56" t="s">
+        <v>16</v>
+      </c>
       <c r="I41" s="56"/>
       <c r="J41" s="56"/>
       <c r="K41" s="56"/>
       <c r="L41" s="16"/>
     </row>
-    <row r="42" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="42"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23"/>
+    <row r="42" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="23"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
       <c r="L42" s="16"/>
     </row>
     <row r="43" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1754,46 +1754,46 @@
       <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
-      <c r="H47" s="28"/>
+      <c r="H47" s="44"/>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
-      <c r="K47" s="29"/>
+      <c r="K47" s="23"/>
       <c r="L47" s="16"/>
     </row>
     <row r="48" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="53" t="s">
-        <v>21</v>
-      </c>
+      <c r="A48" s="53"/>
       <c r="B48" s="53"/>
       <c r="C48" s="53"/>
       <c r="D48" s="53"/>
       <c r="E48" s="53"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
-      <c r="H48" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="29"/>
       <c r="L48" s="16"/>
     </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
-      <c r="H49" s="54"/>
+      <c r="H49" s="54" t="s">
+        <v>28</v>
+      </c>
       <c r="I49" s="54"/>
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
@@ -1814,35 +1814,31 @@
       <c r="L50" s="16"/>
     </row>
     <row r="51" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="54"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
+      <c r="A51" s="55"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="I51" s="52"/>
-      <c r="J51" s="52"/>
-      <c r="K51" s="52"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="54"/>
       <c r="L51" s="16"/>
     </row>
     <row r="52" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="52"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
+      <c r="A52" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
       <c r="H52" s="52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I52" s="52"/>
       <c r="J52" s="52"/>
@@ -1851,49 +1847,53 @@
     </row>
     <row r="53" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="52"/>
       <c r="C53" s="52"/>
       <c r="D53" s="52"/>
       <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
+      <c r="F53" s="24"/>
       <c r="G53" s="24"/>
       <c r="H53" s="52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I53" s="52"/>
       <c r="J53" s="52"/>
       <c r="K53" s="52"/>
       <c r="L53" s="16"/>
     </row>
-    <row r="54" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
+    <row r="54" spans="1:12" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="52"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="I54" s="52"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="52"/>
       <c r="L54" s="16"/>
     </row>
-    <row r="55" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
+    <row r="55" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
     </row>
     <row r="56" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
@@ -2003,11 +2003,12 @@
       <c r="G63" s="10"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
+      <c r="J63" s="9"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
     </row>
     <row r="64" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
@@ -2097,12 +2098,18 @@
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:12" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B71" s="12"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
+    <row r="71" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
     </row>
     <row r="72" spans="1:12" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
@@ -2174,8 +2181,12 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
+    <row r="82" spans="2:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="12"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
@@ -2206,6 +2217,9 @@
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="50">
@@ -2221,44 +2235,44 @@
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="G12:K12"/>
+    <mergeCell ref="A22:J22"/>
     <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A20:J20"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="H40:K41"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="H41:K42"/>
+    <mergeCell ref="A42:E42"/>
     <mergeCell ref="A29:K29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:E36"/>
     <mergeCell ref="A37:K37"/>
     <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="H49:K51"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A51:E51"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="H52:K52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="H48:K50"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="H51:K51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="10" orientation="portrait" r:id="rId1"/>

</xml_diff>